<commit_message>
Add image upload functionality to CsRecordModel; update forms and views for SLMon image handling
</commit_message>
<xml_diff>
--- a/cl_seiscomp/static/cl_seiscomp/cl_seiscomp.xlsx
+++ b/cl_seiscomp/static/cl_seiscomp/cl_seiscomp.xlsx
@@ -3988,138 +3988,138 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="27">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="30">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="31">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="30">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="32">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="34">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+  <cellXfs count="67">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4163,7 +4163,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4173,7 +4173,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4191,13 +4191,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4209,15 +4209,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4253,7 +4253,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4263,7 +4263,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4275,7 +4274,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4908,8 +4906,8 @@
   </sheetPr>
   <dimension ref="A1:S1137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="Q254" sqref="Q254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4814814814815" defaultRowHeight="14.4"/>
@@ -13229,7 +13227,7 @@
       <c r="M265" s="39"/>
       <c r="N265" s="60"/>
       <c r="O265" s="60"/>
-      <c r="P265" s="62"/>
+      <c r="P265" s="28"/>
     </row>
     <row r="266" ht="14.25" customHeight="1" spans="1:16">
       <c r="A266" s="16">
@@ -13249,11 +13247,11 @@
         <v>1022</v>
       </c>
       <c r="K266" s="28"/>
-      <c r="L266" s="63"/>
+      <c r="L266" s="62"/>
       <c r="M266" s="39"/>
-      <c r="N266" s="63"/>
-      <c r="O266" s="63"/>
-      <c r="P266" s="62"/>
+      <c r="N266" s="62"/>
+      <c r="O266" s="62"/>
+      <c r="P266" s="28"/>
     </row>
     <row r="267" ht="14.25" customHeight="1" spans="1:16">
       <c r="A267" s="16">
@@ -13270,14 +13268,14 @@
       <c r="F267" s="19"/>
       <c r="G267" s="10"/>
       <c r="H267" s="55"/>
-      <c r="I267" s="64"/>
-      <c r="J267" s="64"/>
-      <c r="K267" s="65"/>
-      <c r="L267" s="63"/>
-      <c r="M267" s="66"/>
-      <c r="N267" s="67"/>
-      <c r="O267" s="67"/>
-      <c r="P267" s="68"/>
+      <c r="I267" s="63"/>
+      <c r="J267" s="63"/>
+      <c r="K267" s="64"/>
+      <c r="L267" s="62"/>
+      <c r="M267" s="65"/>
+      <c r="N267" s="66"/>
+      <c r="O267" s="66"/>
+      <c r="P267" s="64"/>
     </row>
     <row r="268" ht="14.25" customHeight="1" spans="1:16">
       <c r="A268" s="16">

</xml_diff>

<commit_message>
Fix range in Excel export functions to iterate through rows 7 to 249
</commit_message>
<xml_diff>
--- a/cl_seiscomp/static/cl_seiscomp/cl_seiscomp.xlsx
+++ b/cl_seiscomp/static/cl_seiscomp/cl_seiscomp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9995" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="10440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="checklist_seiscomp" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="1032">
   <si>
     <t>KONDISI  STASIUN  SEISCOMP6</t>
   </si>
@@ -1707,10 +1707,10 @@
     <t>Jangkat,Merangin</t>
   </si>
   <si>
-    <t>SPSI</t>
-  </si>
-  <si>
-    <t>Sidrap</t>
+    <t>SPSJM</t>
+  </si>
+  <si>
+    <t>Serang-Panjang</t>
   </si>
   <si>
     <t>JPJI</t>
@@ -1719,10 +1719,10 @@
     <t>Jatiluhur,Purwakarta</t>
   </si>
   <si>
-    <t>SPSJM</t>
-  </si>
-  <si>
-    <t>Serang-Panjang</t>
+    <t>SPSM</t>
+  </si>
+  <si>
+    <t>Sitellu-Tali-UrangJulu,Pakpak-Bharat</t>
   </si>
   <si>
     <t>JPSI</t>
@@ -1731,10 +1731,10 @@
     <t>Jurai,Pesisir-Selatan</t>
   </si>
   <si>
-    <t>SPSM</t>
-  </si>
-  <si>
-    <t>Sitellu-Tali-UrangJulu,Pakpak-Bharat</t>
+    <t>SRBI</t>
+  </si>
+  <si>
+    <t>Singaraja</t>
   </si>
   <si>
     <t>JSBFM</t>
@@ -1743,10 +1743,10 @@
     <t>Jereweh</t>
   </si>
   <si>
-    <t>SRBI</t>
-  </si>
-  <si>
-    <t>Singaraja</t>
+    <t>SRMI</t>
+  </si>
+  <si>
+    <t>Seram-Utara,MalukuTengah</t>
   </si>
   <si>
     <t>JTJM</t>
@@ -1755,10 +1755,10 @@
     <t>Jampang-Tengah,Sukabumi</t>
   </si>
   <si>
-    <t>SRMI</t>
-  </si>
-  <si>
-    <t>Seram-Utara,MalukuTengah</t>
+    <t>SRPI</t>
+  </si>
+  <si>
+    <t>Serui</t>
   </si>
   <si>
     <t>JWJM</t>
@@ -1767,10 +1767,10 @@
     <t>Juwangi,Boyolali</t>
   </si>
   <si>
-    <t>SRPI</t>
-  </si>
-  <si>
-    <t>Serui</t>
+    <t>SRSI</t>
+  </si>
+  <si>
+    <t>Sorowako</t>
   </si>
   <si>
     <t>KABKI</t>
@@ -1779,10 +1779,10 @@
     <t>Bongan,KutaiBarat</t>
   </si>
   <si>
-    <t>SRSI</t>
-  </si>
-  <si>
-    <t>Sorowako</t>
+    <t>SSASI</t>
+  </si>
+  <si>
+    <t>Simeulue Barat,Simeulue</t>
   </si>
   <si>
     <t>KAKKI</t>
@@ -1791,10 +1791,10 @@
     <t>Karangan,KutaiTimur</t>
   </si>
   <si>
-    <t>SSASI</t>
-  </si>
-  <si>
-    <t>Simeulue Barat,Simeulue</t>
+    <t>SSJM</t>
+  </si>
+  <si>
+    <t>Sukaraja,Sukabumi</t>
   </si>
   <si>
     <t>KAPI</t>
@@ -1803,10 +1803,10 @@
     <t>Kappang</t>
   </si>
   <si>
-    <t>SSJM</t>
-  </si>
-  <si>
-    <t>Sukaraja,Sukabumi</t>
+    <t>SSKI</t>
+  </si>
+  <si>
+    <t>Singkawang</t>
   </si>
   <si>
     <t>KARPI</t>
@@ -1815,10 +1815,10 @@
     <t>Kabare,RajaAmpat</t>
   </si>
   <si>
-    <t>SSKI</t>
-  </si>
-  <si>
-    <t>Singkawang</t>
+    <t>SSMI</t>
+  </si>
+  <si>
+    <t>Siritaun-WidaTimur,Seram-Bagian-Timur</t>
   </si>
   <si>
     <t>KASAI</t>
@@ -1827,10 +1827,10 @@
     <t>Kota-Baharu,Aceh-Singkil</t>
   </si>
   <si>
-    <t>SSMI</t>
-  </si>
-  <si>
-    <t>Siritaun-WidaTimur,Seram-Bagian-Timur</t>
+    <t>SSSI</t>
+  </si>
+  <si>
+    <t>Subulussalam</t>
   </si>
   <si>
     <t>KBBI</t>
@@ -1839,10 +1839,10 @@
     <t>Kintamani,Bangli</t>
   </si>
   <si>
-    <t>SSSI</t>
-  </si>
-  <si>
-    <t>Subulussalam</t>
+    <t>SSSM</t>
+  </si>
+  <si>
+    <t>Sangir,Solok-Selatan</t>
   </si>
   <si>
     <t>KBJM</t>
@@ -1851,10 +1851,10 @@
     <t>Kunduran,Blora</t>
   </si>
   <si>
-    <t>SSSM</t>
-  </si>
-  <si>
-    <t>Sangir,Solok-Selatan</t>
+    <t>STSI</t>
+  </si>
+  <si>
+    <t>Silaut,Pesisir-Selatan</t>
   </si>
   <si>
     <t>KBKI</t>
@@ -1863,10 +1863,10 @@
     <t>Kotabaru</t>
   </si>
   <si>
-    <t>STSI</t>
-  </si>
-  <si>
-    <t>Silaut,Pesisir-Selatan</t>
+    <t>SUPJI</t>
+  </si>
+  <si>
+    <t>Sumur,Pandeglang</t>
   </si>
   <si>
     <t>KBSSI</t>
@@ -1875,10 +1875,10 @@
     <t>Kodi Bangedo,Sumba Barat Daya</t>
   </si>
   <si>
-    <t>SUPJI</t>
-  </si>
-  <si>
-    <t>Sumur,Pandeglang</t>
+    <t>SUSM</t>
+  </si>
+  <si>
+    <t>Sekincau,Lampung-Barat</t>
   </si>
   <si>
     <t>KDI</t>
@@ -1887,10 +1887,10 @@
     <t>Kendari</t>
   </si>
   <si>
-    <t>SUSM</t>
-  </si>
-  <si>
-    <t>Sekincau,Lampung-Barat</t>
+    <t>SUSPI</t>
+  </si>
+  <si>
+    <t>SupioriTimur,Supiori</t>
   </si>
   <si>
     <t>KGCM</t>
@@ -1899,10 +1899,10 @@
     <t>Kwandang,Gorontalo</t>
   </si>
   <si>
-    <t>SUSPI</t>
-  </si>
-  <si>
-    <t>SupioriTimur,Supiori</t>
+    <t>SWCM</t>
+  </si>
+  <si>
+    <t>Sabbang-Paru,Wajo</t>
   </si>
   <si>
     <t>KHK</t>
@@ -1911,10 +1911,7 @@
     <t>Kahang-Kahang</t>
   </si>
   <si>
-    <t>SWCM</t>
-  </si>
-  <si>
-    <t>Sabbang-Paru,Wajo</t>
+    <t>SWI</t>
   </si>
   <si>
     <t>KHSSI</t>
@@ -1923,7 +1920,7 @@
     <t>KatalaHamuLingu,SumbaTimur</t>
   </si>
   <si>
-    <t>SWI</t>
+    <t>SWJI</t>
   </si>
   <si>
     <t>KIMPI</t>
@@ -1932,7 +1929,10 @@
     <t>Kimaam,Merauke</t>
   </si>
   <si>
-    <t>SWJI</t>
+    <t>SWPM</t>
+  </si>
+  <si>
+    <t>Sidey,Manokwari</t>
   </si>
   <si>
     <t>KJCM</t>
@@ -1941,10 +1941,10 @@
     <t>Kelara</t>
   </si>
   <si>
-    <t>SWPM</t>
-  </si>
-  <si>
-    <t>Sidey,Manokwari</t>
+    <t>SYJI</t>
+  </si>
+  <si>
+    <t>Candi-Abang,Berbah,Sleman</t>
   </si>
   <si>
     <t>KKJM</t>
@@ -1953,10 +1953,10 @@
     <t>Kokap,KulonProgo</t>
   </si>
   <si>
-    <t>SYJI</t>
-  </si>
-  <si>
-    <t>Candi-Abang,Berbah,Sleman</t>
+    <t>TAGJI</t>
+  </si>
+  <si>
+    <t>Tanjungsari,Gunungkidul</t>
   </si>
   <si>
     <t>KKKI</t>
@@ -1965,10 +1965,10 @@
     <t>Kendawangan</t>
   </si>
   <si>
-    <t>TAGJI</t>
-  </si>
-  <si>
-    <t>Tanjungsari,Gunungkidul</t>
+    <t>TAMI</t>
+  </si>
+  <si>
+    <t>Teluk-Ambon,KotaAmbon</t>
   </si>
   <si>
     <t>KKKKI</t>
@@ -1977,10 +1977,10 @@
     <t>Katingan-Kuala,Katingan</t>
   </si>
   <si>
-    <t>TAMI</t>
-  </si>
-  <si>
-    <t>Teluk-Ambon,KotaAmbon</t>
+    <t>TAPSI</t>
+  </si>
+  <si>
+    <t>Tapango,PolewaliMandar</t>
   </si>
   <si>
     <t>KKMI</t>
@@ -1989,10 +1989,10 @@
     <t>Kei-Kecil,MalukuTenggara</t>
   </si>
   <si>
-    <t>TAPSI</t>
-  </si>
-  <si>
-    <t>Tapango,PolewaliMandar</t>
+    <t>TARAI</t>
+  </si>
+  <si>
+    <t>Tarakan</t>
   </si>
   <si>
     <t>KKSI</t>
@@ -2001,10 +2001,10 @@
     <t>Kolaka</t>
   </si>
   <si>
-    <t>TARAI</t>
-  </si>
-  <si>
-    <t>Tarakan</t>
+    <t>TASI</t>
+  </si>
+  <si>
+    <t>Tanjung-Raya,Agam</t>
   </si>
   <si>
     <t>KKTKI</t>
@@ -2013,10 +2013,10 @@
     <t>Kombeng,Kutai-Timur</t>
   </si>
   <si>
-    <t>TASI</t>
-  </si>
-  <si>
-    <t>Tanjung-Raya,Agam</t>
+    <t>TASSI</t>
+  </si>
+  <si>
+    <t>Tagulandang SiauTagulandangBiaro</t>
   </si>
   <si>
     <t>KLI</t>
@@ -2025,10 +2025,10 @@
     <t>Kotabumi</t>
   </si>
   <si>
-    <t>TASSI</t>
-  </si>
-  <si>
-    <t>Tagulandang SiauTagulandangBiaro</t>
+    <t>TBCM</t>
+  </si>
+  <si>
+    <t>Tonra,Bone</t>
   </si>
   <si>
     <t>KLJI</t>
@@ -2037,10 +2037,10 @@
     <t>Klakah,Lumajang</t>
   </si>
   <si>
-    <t>TBCM</t>
-  </si>
-  <si>
-    <t>Tonra,Bone</t>
+    <t>TBJI</t>
+  </si>
+  <si>
+    <t>Tambak-Boyo</t>
   </si>
   <si>
     <t>KLNI</t>
@@ -2049,19 +2049,19 @@
     <t>Mataram,Plombok</t>
   </si>
   <si>
-    <t>TBJI</t>
-  </si>
-  <si>
-    <t>Tambak-Boyo</t>
+    <t>TBJKI</t>
+  </si>
+  <si>
+    <t>Jaro,Tabalong</t>
   </si>
   <si>
     <t>KLSI</t>
   </si>
   <si>
-    <t>TBJKI</t>
-  </si>
-  <si>
-    <t>Jaro,Tabalong</t>
+    <t>TBKI</t>
+  </si>
+  <si>
+    <t>Teluk-Bayur,Berau</t>
   </si>
   <si>
     <t>KLSM</t>
@@ -2070,10 +2070,10 @@
     <t>Kluet-Utara,Aceh-Selatan</t>
   </si>
   <si>
-    <t>TBKI</t>
-  </si>
-  <si>
-    <t>Teluk-Bayur,Berau</t>
+    <t>TBMCM</t>
+  </si>
+  <si>
+    <t>Tutuyan,BolaangTimur,Mongondow</t>
   </si>
   <si>
     <t>KMBFM</t>
@@ -2082,10 +2082,10 @@
     <t>Kuwus,ManggaraiBarat</t>
   </si>
   <si>
-    <t>TBMCM</t>
-  </si>
-  <si>
-    <t>Tutuyan,BolaangTimur,Mongondow</t>
+    <t>TBMUI</t>
+  </si>
+  <si>
+    <t>TaliabuBarat,PulauTaliabu</t>
   </si>
   <si>
     <t>KMMI</t>
@@ -2094,10 +2094,10 @@
     <t>Kalianget</t>
   </si>
   <si>
-    <t>TBMUI</t>
-  </si>
-  <si>
-    <t>TaliabuBarat,PulauTaliabu</t>
+    <t>TDNI</t>
+  </si>
+  <si>
+    <t>Teluk-Dalam,Pulau-Nias</t>
   </si>
   <si>
     <t>KMNI</t>
@@ -2106,10 +2106,10 @@
     <t>Kota-Mataram</t>
   </si>
   <si>
-    <t>TDNI</t>
-  </si>
-  <si>
-    <t>Teluk-Dalam,Pulau-Nias</t>
+    <t>TEBBI</t>
+  </si>
+  <si>
+    <t>Tejakula,Buleleng</t>
   </si>
   <si>
     <t>KMPI</t>
@@ -2118,10 +2118,10 @@
     <t>Kaimana</t>
   </si>
   <si>
-    <t>TEBBI</t>
-  </si>
-  <si>
-    <t>Tejakula,Buleleng</t>
+    <t>TGCM</t>
+  </si>
+  <si>
+    <t>Telaga,Gorontalo</t>
   </si>
   <si>
     <t>KMSI</t>
@@ -2130,10 +2130,10 @@
     <t>Kotamubagu</t>
   </si>
   <si>
-    <t>TGCM</t>
-  </si>
-  <si>
-    <t>Telaga,Gorontalo</t>
+    <t>TIKSI</t>
+  </si>
+  <si>
+    <t>Tinondo, Kolaka Timur,</t>
   </si>
   <si>
     <t>KOMFI</t>
@@ -2142,10 +2142,10 @@
     <t>Komodo,Manggarai Barat</t>
   </si>
   <si>
-    <t>TIKSI</t>
-  </si>
-  <si>
-    <t>Tinondo, Kolaka Timur,</t>
+    <t>TIPSI</t>
+  </si>
+  <si>
+    <t>Tinombo, Parigi Moutong,</t>
   </si>
   <si>
     <t>KORPI</t>
@@ -2154,10 +2154,10 @@
     <t>Kofiau,RajaAmpat</t>
   </si>
   <si>
-    <t>TIPSI</t>
-  </si>
-  <si>
-    <t>Tinombo, Parigi Moutong,</t>
+    <t>TKSM</t>
+  </si>
+  <si>
+    <t>Tiganderket,Karo</t>
   </si>
   <si>
     <t>KPJI</t>
@@ -2166,10 +2166,10 @@
     <t>Karang-Pucung</t>
   </si>
   <si>
-    <t>TKSM</t>
-  </si>
-  <si>
-    <t>Tiganderket,Karo</t>
+    <t>TLCM</t>
+  </si>
+  <si>
+    <t>Tomoni,Luwu-Timur</t>
   </si>
   <si>
     <t>KPJM</t>
@@ -2178,10 +2178,10 @@
     <t>Kapas,Bojonegoro</t>
   </si>
   <si>
-    <t>TLCM</t>
-  </si>
-  <si>
-    <t>Tomoni,Luwu-Timur</t>
+    <t>TLE2</t>
+  </si>
+  <si>
+    <t>Tual,Kai</t>
   </si>
   <si>
     <t>KRAI</t>
@@ -2190,10 +2190,10 @@
     <t>Kairatu,SeramBagianBarat</t>
   </si>
   <si>
-    <t>TLE2</t>
-  </si>
-  <si>
-    <t>Tual,Kai</t>
+    <t>TMSI</t>
+  </si>
+  <si>
+    <t>Tondano</t>
   </si>
   <si>
     <t>KRJI</t>
@@ -2202,10 +2202,10 @@
     <t>Kerinci</t>
   </si>
   <si>
-    <t>TMSI</t>
-  </si>
-  <si>
-    <t>Tondano</t>
+    <t>TMSM</t>
+  </si>
+  <si>
+    <t>Teramang-Jaya,Mukomuko</t>
   </si>
   <si>
     <t>KRSI</t>
@@ -2214,10 +2214,10 @@
     <t>Karosa</t>
   </si>
   <si>
-    <t>TMSM</t>
-  </si>
-  <si>
-    <t>Teramang-Jaya,Mukomuko</t>
+    <t>TMTMM</t>
+  </si>
+  <si>
+    <t>Tehoru,MalukuTengah</t>
   </si>
   <si>
     <t>KSI</t>
@@ -2226,10 +2226,10 @@
     <t>Kepahiang</t>
   </si>
   <si>
-    <t>TMTMM</t>
-  </si>
-  <si>
-    <t>Tehoru,MalukuTengah</t>
+    <t>TNGI</t>
+  </si>
+  <si>
+    <t>Tangerang</t>
   </si>
   <si>
     <t>KTMI</t>
@@ -2238,10 +2238,10 @@
     <t>Kormomolin,Kepulauan-Tanimbar</t>
   </si>
   <si>
-    <t>TNGI</t>
-  </si>
-  <si>
-    <t>Tangerang</t>
+    <t>TNTI</t>
+  </si>
+  <si>
+    <t>Ternate</t>
   </si>
   <si>
     <t>KTTI</t>
@@ -2250,10 +2250,10 @@
     <t>Kolbano,Timor-TengahSelatan</t>
   </si>
   <si>
-    <t>TNTI</t>
-  </si>
-  <si>
-    <t>Ternate</t>
+    <t>TOBSI</t>
+  </si>
+  <si>
+    <t>Toili,Banggai</t>
   </si>
   <si>
     <t>KUBSI</t>
@@ -2262,10 +2262,10 @@
     <t>Kulisusu,ButonUtara</t>
   </si>
   <si>
-    <t>TOBSI</t>
-  </si>
-  <si>
-    <t>Toili,Banggai</t>
+    <t>TOCM</t>
+  </si>
+  <si>
+    <t>Towuti,Luwu-Timur</t>
   </si>
   <si>
     <t>KUKI</t>
@@ -2274,10 +2274,10 @@
     <t>Kutai-Barat</t>
   </si>
   <si>
-    <t>TOCM</t>
-  </si>
-  <si>
-    <t>Towuti,Luwu-Timur</t>
+    <t>TOJI</t>
+  </si>
+  <si>
+    <t>Tomo,Sumedang</t>
   </si>
   <si>
     <t>KUSI</t>
@@ -2286,10 +2286,10 @@
     <t>Kluet-Tengah,AcehSelatan</t>
   </si>
   <si>
-    <t>TOJI</t>
-  </si>
-  <si>
-    <t>Tomo,Sumedang</t>
+    <t>TOLI2</t>
+  </si>
+  <si>
+    <t>Tolitoli</t>
   </si>
   <si>
     <t>KWJI</t>
@@ -2298,10 +2298,10 @@
     <t>Kertek,Wonosobo</t>
   </si>
   <si>
-    <t>TOLI2</t>
-  </si>
-  <si>
-    <t>Tolitoli</t>
+    <t>TOTSI</t>
+  </si>
+  <si>
+    <t>Tojo,TojoUna-Una</t>
   </si>
   <si>
     <t>LASI</t>
@@ -2310,10 +2310,10 @@
     <t>Langsa</t>
   </si>
   <si>
-    <t>TOTSI</t>
-  </si>
-  <si>
-    <t>Tojo,TojoUna-Una</t>
+    <t>TPCI</t>
+  </si>
+  <si>
+    <t>Taopa,Parigi-Moutong</t>
   </si>
   <si>
     <t>LBFI</t>
@@ -2322,10 +2322,10 @@
     <t>Labuhan-Bajo</t>
   </si>
   <si>
-    <t>TPCI</t>
-  </si>
-  <si>
-    <t>Taopa,Parigi-Moutong</t>
+    <t>TPI</t>
+  </si>
+  <si>
+    <t>Tanjung-Pandan,Belitung</t>
   </si>
   <si>
     <t>LBNFM</t>
@@ -2334,10 +2334,10 @@
     <t>Lambu</t>
   </si>
   <si>
-    <t>TPI</t>
-  </si>
-  <si>
-    <t>Tanjung-Pandan,Belitung</t>
+    <t>TPRI</t>
+  </si>
+  <si>
+    <t>Tanjung-Pinang</t>
   </si>
   <si>
     <t>LBTSI</t>
@@ -2346,10 +2346,10 @@
     <t>Lintau Buo Utara,Tanah Datar</t>
   </si>
   <si>
-    <t>TPRI</t>
-  </si>
-  <si>
-    <t>Tanjung-Pinang</t>
+    <t>TPSI</t>
+  </si>
+  <si>
+    <t>Tangse,Pidie</t>
   </si>
   <si>
     <t>LDSI</t>
@@ -2358,10 +2358,10 @@
     <t>Sukandebi</t>
   </si>
   <si>
-    <t>TPSI</t>
-  </si>
-  <si>
-    <t>Tangse,Pidie</t>
+    <t>TPTI</t>
+  </si>
+  <si>
+    <t>Tapak-Tuan</t>
   </si>
   <si>
     <t>LEM</t>
@@ -2370,10 +2370,10 @@
     <t>Lembang</t>
   </si>
   <si>
-    <t>TPTI</t>
-  </si>
-  <si>
-    <t>Tapak-Tuan</t>
+    <t>TRIYO</t>
+  </si>
+  <si>
+    <t>Sipora-Selatan,Kep.-Mentawai</t>
   </si>
   <si>
     <t>LEMFI</t>
@@ -2382,10 +2382,10 @@
     <t>Lembor, Manggarai Barat</t>
   </si>
   <si>
-    <t>TRIYO</t>
-  </si>
-  <si>
-    <t>Sipora-Selatan,Kep.-Mentawai</t>
+    <t>TRPI</t>
+  </si>
+  <si>
+    <t>Tanah-Merah</t>
   </si>
   <si>
     <t>LESM</t>
@@ -2394,10 +2394,10 @@
     <t>Lemong,Pesisir-Barat</t>
   </si>
   <si>
-    <t>TRPI</t>
-  </si>
-  <si>
-    <t>Tanah-Merah</t>
+    <t>TSI</t>
+  </si>
+  <si>
+    <t>Tuntungan</t>
   </si>
   <si>
     <t>LHMI</t>
@@ -2406,10 +2406,10 @@
     <t>Lhokseumawe</t>
   </si>
   <si>
-    <t>TSI</t>
-  </si>
-  <si>
-    <t>Tuntungan</t>
+    <t>TSJM</t>
+  </si>
+  <si>
+    <t>Tanjungsiang,Subang</t>
   </si>
   <si>
     <t>LHSM</t>
@@ -2418,10 +2418,10 @@
     <t>Semendo,Lahat</t>
   </si>
   <si>
-    <t>TSJM</t>
-  </si>
-  <si>
-    <t>Tanjungsiang,Subang</t>
+    <t>TSNI</t>
+  </si>
+  <si>
+    <t>Tarano</t>
   </si>
   <si>
     <t>LISM</t>
@@ -2430,10 +2430,10 @@
     <t>Lingge-Isaq,Aceh-Tengah</t>
   </si>
   <si>
-    <t>TSNI</t>
-  </si>
-  <si>
-    <t>Tarano</t>
+    <t>TSPI</t>
+  </si>
+  <si>
+    <t>Teminabuan,Sorong-Selatan</t>
   </si>
   <si>
     <t>LJPI</t>
@@ -2442,10 +2442,10 @@
     <t>Lereh,Jayapura</t>
   </si>
   <si>
-    <t>TSPI</t>
-  </si>
-  <si>
-    <t>Teminabuan,Sorong-Selatan</t>
+    <t>TTPSI</t>
+  </si>
+  <si>
+    <t>Tondong-Talasa,Pangkep</t>
   </si>
   <si>
     <t>LKCI</t>
@@ -2454,10 +2454,10 @@
     <t>Lasusua,Lasusua</t>
   </si>
   <si>
-    <t>TTPSI</t>
-  </si>
-  <si>
-    <t>Tondong-Talasa,Pangkep</t>
+    <t>TTSI</t>
+  </si>
+  <si>
+    <t>Tana-Toraja</t>
   </si>
   <si>
     <t>LKSM</t>
@@ -2466,10 +2466,10 @@
     <t>Suliki,Limapuluh-Koto</t>
   </si>
   <si>
-    <t>TTSI</t>
-  </si>
-  <si>
-    <t>Tana-Toraja</t>
+    <t>TTSM</t>
+  </si>
+  <si>
+    <t>Tano-Tombangan-Angkola,TapanuliSelatan</t>
   </si>
   <si>
     <t>LKUCM</t>
@@ -2478,10 +2478,10 @@
     <t>Langgikima</t>
   </si>
   <si>
-    <t>TTSM</t>
-  </si>
-  <si>
-    <t>Tano-Tombangan-Angkola,TapanuliSelatan</t>
+    <t>TTSMI</t>
+  </si>
+  <si>
+    <t>TaniwelTimur,SeramBagianBarat</t>
   </si>
   <si>
     <t>LLSI</t>
@@ -2490,10 +2490,10 @@
     <t>Lubuk-LinggauBarat,Kota-Lubuk-Linggau</t>
   </si>
   <si>
-    <t>TTSMI</t>
-  </si>
-  <si>
-    <t>TaniwelTimur,SeramBagianBarat</t>
+    <t>TUJI</t>
+  </si>
+  <si>
+    <t>Tumpakrejo,Jember</t>
   </si>
   <si>
     <t>LLSM</t>
@@ -2502,10 +2502,10 @@
     <t>Limau,Tanggamus</t>
   </si>
   <si>
-    <t>TUJI</t>
-  </si>
-  <si>
-    <t>Tumpakrejo,Jember</t>
+    <t>UGM</t>
+  </si>
+  <si>
+    <t>Wanagama</t>
   </si>
   <si>
     <t>LMNI</t>
@@ -2514,10 +2514,10 @@
     <t>Lembata</t>
   </si>
   <si>
-    <t>UGM</t>
-  </si>
-  <si>
-    <t>Wanagama</t>
+    <t>UKCM</t>
+  </si>
+  <si>
+    <t>Unaaha</t>
   </si>
   <si>
     <t>LMTI</t>
@@ -2526,10 +2526,10 @@
     <t>Langke-Rembong,Manggarai</t>
   </si>
   <si>
-    <t>UKCM</t>
-  </si>
-  <si>
-    <t>Unaaha</t>
+    <t>ULMSI</t>
+  </si>
+  <si>
+    <t>Ulumanda,Majene</t>
   </si>
   <si>
     <t>LOCM</t>
@@ -2538,10 +2538,10 @@
     <t>Lore-Tengah,Poso</t>
   </si>
   <si>
-    <t>ULMSI</t>
-  </si>
-  <si>
-    <t>Ulumanda,Majene</t>
+    <t>ULSM</t>
+  </si>
+  <si>
+    <t>Ulu-Musi,Empat-Lawang</t>
   </si>
   <si>
     <t>LOMSI</t>
@@ -2550,10 +2550,10 @@
     <t>Lohia,Muna</t>
   </si>
   <si>
-    <t>ULSM</t>
-  </si>
-  <si>
-    <t>Ulu-Musi,Empat-Lawang</t>
+    <t>UMKSI</t>
+  </si>
+  <si>
+    <t>Ujan Mas,Kepahiang</t>
   </si>
   <si>
     <t>LPCM</t>
@@ -2562,10 +2562,10 @@
     <t>Lembang,Pinrang</t>
   </si>
   <si>
-    <t>UMKSI</t>
-  </si>
-  <si>
-    <t>Ujan Mas,Kepahiang</t>
+    <t>UMSSI</t>
+  </si>
+  <si>
+    <t>Umalulu,SumbaTimur</t>
   </si>
   <si>
     <t>LPSM</t>
@@ -2574,10 +2574,10 @@
     <t>Lengayang,Pesisir-Selatan</t>
   </si>
   <si>
-    <t>UMSSI</t>
-  </si>
-  <si>
-    <t>Umalulu,SumbaTimur</t>
+    <t>USFM</t>
+  </si>
+  <si>
+    <t>Utan</t>
   </si>
   <si>
     <t>LRTI</t>
@@ -2586,10 +2586,10 @@
     <t>Larantuka</t>
   </si>
   <si>
-    <t>USFM</t>
-  </si>
-  <si>
-    <t>Utan</t>
+    <t>USTI</t>
+  </si>
+  <si>
+    <t>Umbu-RatuNggay,Sumba-Tengah</t>
   </si>
   <si>
     <t>LSCM</t>
@@ -2598,10 +2598,10 @@
     <t>Lalabati-Rilau,Soppeng</t>
   </si>
   <si>
-    <t>USTI</t>
-  </si>
-  <si>
-    <t>Umbu-RatuNggay,Sumba-Tengah</t>
+    <t>UTSI</t>
+  </si>
+  <si>
+    <t>Ulu-Belu,Tanggamus</t>
   </si>
   <si>
     <t>LSNI</t>
@@ -2610,10 +2610,10 @@
     <t>Lunyuk,Sumbawa</t>
   </si>
   <si>
-    <t>UTSI</t>
-  </si>
-  <si>
-    <t>Ulu-Belu,Tanggamus</t>
+    <t>UTSM</t>
+  </si>
+  <si>
+    <t>Ulu-Talo,Seluma</t>
   </si>
   <si>
     <t>LTNI</t>
@@ -2622,10 +2622,10 @@
     <t>Lombok-Timur</t>
   </si>
   <si>
-    <t>UTSM</t>
-  </si>
-  <si>
-    <t>Ulu-Talo,Seluma</t>
+    <t>UTUSI</t>
+  </si>
+  <si>
+    <t>Una-Una,Tojo-Una-Una</t>
   </si>
   <si>
     <t>LTNSI</t>
@@ -2634,10 +2634,10 @@
     <t>Lahewa Timur,Nias Utara</t>
   </si>
   <si>
-    <t>UTUSI</t>
-  </si>
-  <si>
-    <t>Una-Una,Tojo-Una-Una</t>
+    <t>UWJI</t>
+  </si>
+  <si>
+    <t>Ujung-Watu</t>
   </si>
   <si>
     <t>LTSM</t>
@@ -2646,10 +2646,10 @@
     <t>Lumut,Tapanuli-Tengah</t>
   </si>
   <si>
-    <t>UWJI</t>
-  </si>
-  <si>
-    <t>Ujung-Watu</t>
+    <t>UWNPI</t>
+  </si>
+  <si>
+    <t>Uwapa,Nabire</t>
   </si>
   <si>
     <t>LUCM</t>
@@ -2658,10 +2658,10 @@
     <t>Lore-Utara,Poso</t>
   </si>
   <si>
-    <t>UWNPI</t>
-  </si>
-  <si>
-    <t>Uwapa,Nabire</t>
+    <t>WAMI</t>
+  </si>
+  <si>
+    <t>Wamena</t>
   </si>
   <si>
     <t>LUJI</t>
@@ -2670,10 +2670,10 @@
     <t>Lumbang,Pasuruan</t>
   </si>
   <si>
-    <t>WAMI</t>
-  </si>
-  <si>
-    <t>Wamena</t>
+    <t>WANPI</t>
+  </si>
+  <si>
+    <t>Wanggar,Nabire</t>
   </si>
   <si>
     <t>LUWI</t>
@@ -2682,10 +2682,10 @@
     <t>Luwuk</t>
   </si>
   <si>
-    <t>WANPI</t>
-  </si>
-  <si>
-    <t>Wanggar,Nabire</t>
+    <t>WBMI</t>
+  </si>
+  <si>
+    <t>Weda-Barat,HalmaheraTengah</t>
   </si>
   <si>
     <t>MABKI</t>
@@ -2694,10 +2694,10 @@
     <t>Maratua,Berau</t>
   </si>
   <si>
-    <t>WBMI</t>
-  </si>
-  <si>
-    <t>Weda-Barat,HalmaheraTengah</t>
+    <t>WBNI</t>
+  </si>
+  <si>
+    <t>Wera,Bima</t>
   </si>
   <si>
     <t>MAKBI</t>
@@ -2706,10 +2706,10 @@
     <t>Manggis,Karangasem</t>
   </si>
   <si>
-    <t>WBNI</t>
-  </si>
-  <si>
-    <t>Wera,Bima</t>
+    <t>WBSI</t>
+  </si>
+  <si>
+    <t>Waikabubak,Sumba</t>
   </si>
   <si>
     <t>MAKKI</t>
@@ -2718,10 +2718,10 @@
     <t>Kep.Karimata,KayongUtara</t>
   </si>
   <si>
-    <t>WBSI</t>
-  </si>
-  <si>
-    <t>Waikabubak,Sumba</t>
+    <t>WEFM</t>
+  </si>
+  <si>
+    <t>Wewaria,Ende</t>
   </si>
   <si>
     <t>MASFI</t>
@@ -2730,10 +2730,10 @@
     <t>Magepanda,Sikka</t>
   </si>
   <si>
-    <t>WEFM</t>
-  </si>
-  <si>
-    <t>Wewaria,Ende</t>
+    <t>WFTFM</t>
+  </si>
+  <si>
+    <t>Wulanggitang,FloresTimur</t>
   </si>
   <si>
     <t>MASM</t>
@@ -2742,10 +2742,10 @@
     <t>Masjid-Raya,Aceh-Besar</t>
   </si>
   <si>
-    <t>WFTFM</t>
-  </si>
-  <si>
-    <t>Wulanggitang,FloresTimur</t>
+    <t>WGJM</t>
+  </si>
+  <si>
+    <t>Wringianom,Gresik</t>
   </si>
   <si>
     <t>MASSI</t>
@@ -2754,10 +2754,10 @@
     <t>Marore,KepulauanSangihe</t>
   </si>
   <si>
-    <t>WGJM</t>
-  </si>
-  <si>
-    <t>Wringianom,Gresik</t>
+    <t>WHMI</t>
+  </si>
+  <si>
+    <t>Wasile,Halmahera-Timur</t>
   </si>
   <si>
     <t>MBBI</t>
@@ -2766,10 +2766,10 @@
     <t>Muara-Bungo,Bungo</t>
   </si>
   <si>
-    <t>WHMI</t>
-  </si>
-  <si>
-    <t>Wasile,Halmahera-Timur</t>
+    <t>WKCM</t>
+  </si>
+  <si>
+    <t>Wolo</t>
   </si>
   <si>
     <t>MBJI</t>
@@ -2778,10 +2778,10 @@
     <t>Majalengka-Banjarnegara</t>
   </si>
   <si>
-    <t>WKCM</t>
-  </si>
-  <si>
-    <t>Wolo</t>
+    <t>WLFM</t>
+  </si>
+  <si>
+    <t>Wulandoni,Lembata</t>
   </si>
   <si>
     <t>MBPI</t>
@@ -2790,10 +2790,10 @@
     <t>Manimeri,Teluk-Bintuni</t>
   </si>
   <si>
-    <t>WLFM</t>
-  </si>
-  <si>
-    <t>Wulandoni,Lembata</t>
+    <t>WLJI</t>
+  </si>
+  <si>
+    <t>Wonosalam,Lebak</t>
   </si>
   <si>
     <t>MBRPI</t>
@@ -2802,10 +2802,10 @@
     <t>MisoolBarat,RajaAmpat</t>
   </si>
   <si>
-    <t>WLJI</t>
-  </si>
-  <si>
-    <t>Wonosalam,Lebak</t>
+    <t>WLTFM</t>
+  </si>
+  <si>
+    <t>Wanasaba</t>
   </si>
   <si>
     <t>MBSM</t>
@@ -2814,10 +2814,10 @@
     <t>Marga-Sakti-Seblat,Bengkulu-Utara</t>
   </si>
   <si>
-    <t>WLTFM</t>
-  </si>
-  <si>
-    <t>Wanasaba</t>
+    <t>WMCM</t>
+  </si>
+  <si>
+    <t>Wita-Ponda,Morowali</t>
   </si>
   <si>
     <t>MDSI</t>
@@ -2826,10 +2826,10 @@
     <t>Muara-Dua</t>
   </si>
   <si>
-    <t>WMCM</t>
-  </si>
-  <si>
-    <t>Wita-Ponda,Morowali</t>
+    <t>WOJI</t>
+  </si>
+  <si>
+    <t>Wonogiri</t>
   </si>
   <si>
     <t>MGAI</t>
@@ -2838,10 +2838,10 @@
     <t>Melonguane-Kep-Talaud</t>
   </si>
   <si>
-    <t>WOJI</t>
-  </si>
-  <si>
-    <t>Wonogiri</t>
+    <t>WRJI</t>
+  </si>
+  <si>
+    <t>Curahdami,Bondowoso</t>
   </si>
   <si>
     <t>MIBPI</t>
@@ -2850,10 +2850,10 @@
     <t>Mindiptana,BovenDigoel</t>
   </si>
   <si>
-    <t>WRJI</t>
-  </si>
-  <si>
-    <t>Curahdami,Bondowoso</t>
+    <t>WSHHI</t>
+  </si>
+  <si>
+    <t>MabaSelatan,HalmaheraTimur</t>
   </si>
   <si>
     <t>MIPI</t>
@@ -2862,10 +2862,10 @@
     <t>Mimika-Baru,Mimika</t>
   </si>
   <si>
-    <t>WSHHI</t>
-  </si>
-  <si>
-    <t>MabaSelatan,HalmaheraTimur</t>
+    <t>WSI</t>
+  </si>
+  <si>
+    <t>Stageof-Sumbawa-Timur</t>
   </si>
   <si>
     <t>MISSI</t>
@@ -2874,10 +2874,10 @@
     <t>Miangas,KepulauanTalaud</t>
   </si>
   <si>
-    <t>WSI</t>
-  </si>
-  <si>
-    <t>Stageof-Sumbawa-Timur</t>
+    <t>WSJM</t>
+  </si>
+  <si>
+    <t>Warungkiara,Sukabumi</t>
   </si>
   <si>
     <t>MKBI</t>
@@ -2886,10 +2886,10 @@
     <t>Muko-Muko,Bengkulu</t>
   </si>
   <si>
-    <t>WSJM</t>
-  </si>
-  <si>
-    <t>Warungkiara,Sukabumi</t>
+    <t>WSTMM</t>
+  </si>
+  <si>
+    <t>Werinama</t>
   </si>
   <si>
     <t>MKJM</t>
@@ -2898,10 +2898,10 @@
     <t>Manisrenggo,Klaten</t>
   </si>
   <si>
-    <t>WSTMM</t>
-  </si>
-  <si>
-    <t>Werinama</t>
+    <t>WTKSI</t>
+  </si>
+  <si>
+    <t>WawoniiTimurLaut,KonaweKepulauan</t>
   </si>
   <si>
     <t>MKSM</t>
@@ -2910,10 +2910,10 @@
     <t>Muara-Sahung,Kaur</t>
   </si>
   <si>
-    <t>WTKSI</t>
-  </si>
-  <si>
-    <t>WawoniiTimurLaut,KonaweKepulauan</t>
+    <t>WUPCM</t>
+  </si>
+  <si>
+    <t>Wara-Utara</t>
   </si>
   <si>
     <t>MLJI</t>
@@ -2922,10 +2922,10 @@
     <t>Malang</t>
   </si>
   <si>
-    <t>WUPCM</t>
-  </si>
-  <si>
-    <t>Wara-Utara</t>
+    <t>WWCI</t>
+  </si>
+  <si>
+    <t>Wangi-wangi,Wakatobi</t>
   </si>
   <si>
     <t>MLJM</t>
@@ -2934,10 +2934,10 @@
     <t>Mantup,Lamongan</t>
   </si>
   <si>
-    <t>WWCI</t>
-  </si>
-  <si>
-    <t>Wangi-wangi,Wakatobi</t>
+    <t>WWPI</t>
+  </si>
+  <si>
+    <t>Waropen-Bawah,Waropen</t>
   </si>
   <si>
     <t>MLMMI</t>
@@ -2946,10 +2946,10 @@
     <t>MoaLakor,MalukuBaratDaya</t>
   </si>
   <si>
-    <t>WWPI</t>
-  </si>
-  <si>
-    <t>Waropen-Bawah,Waropen</t>
+    <t>YBYPI</t>
+  </si>
+  <si>
+    <t>YapenBarat,KepulauanYapen</t>
   </si>
   <si>
     <t>MMCI</t>
@@ -2958,22 +2958,16 @@
     <t>Mamasa,Mamasa</t>
   </si>
   <si>
-    <t>YBYPI</t>
-  </si>
-  <si>
-    <t>YapenBarat,KepulauanYapen</t>
+    <t>YOGI</t>
+  </si>
+  <si>
+    <t>Stageof-Sleman</t>
   </si>
   <si>
     <t>MMRI</t>
   </si>
   <si>
     <t>Maumere,Flores</t>
-  </si>
-  <si>
-    <t>YOGI</t>
-  </si>
-  <si>
-    <t>Stageof-Sleman</t>
   </si>
   <si>
     <t>MMSI</t>
@@ -4792,8 +4786,8 @@
   <sheetPr/>
   <dimension ref="A1:S1137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="N256" sqref="N256"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="H251" sqref="H251:R251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4814814814815" defaultRowHeight="14.4"/>
@@ -9919,7 +9913,7 @@
         <v>627</v>
       </c>
       <c r="J161" s="32" t="s">
-        <v>628</v>
+        <v>465</v>
       </c>
       <c r="K161" s="32"/>
       <c r="L161" s="32"/>
@@ -9935,10 +9929,10 @@
         <v>156</v>
       </c>
       <c r="B162" s="24" t="s">
+        <v>628</v>
+      </c>
+      <c r="C162" s="25" t="s">
         <v>629</v>
-      </c>
-      <c r="C162" s="25" t="s">
-        <v>630</v>
       </c>
       <c r="D162" s="22"/>
       <c r="E162" s="22"/>
@@ -9948,10 +9942,10 @@
         <v>418</v>
       </c>
       <c r="I162" s="30" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J162" s="32" t="s">
-        <v>465</v>
+        <v>544</v>
       </c>
       <c r="K162" s="32"/>
       <c r="L162" s="32"/>
@@ -9967,10 +9961,10 @@
         <v>157</v>
       </c>
       <c r="B163" s="24" t="s">
+        <v>631</v>
+      </c>
+      <c r="C163" s="25" t="s">
         <v>632</v>
-      </c>
-      <c r="C163" s="25" t="s">
-        <v>633</v>
       </c>
       <c r="D163" s="22"/>
       <c r="E163" s="22"/>
@@ -9980,10 +9974,10 @@
         <v>419</v>
       </c>
       <c r="I163" s="30" t="s">
+        <v>633</v>
+      </c>
+      <c r="J163" s="32" t="s">
         <v>634</v>
-      </c>
-      <c r="J163" s="32" t="s">
-        <v>544</v>
       </c>
       <c r="K163" s="32"/>
       <c r="L163" s="32"/>
@@ -12782,33 +12776,18 @@
       <c r="E250" s="22"/>
       <c r="F250" s="22"/>
       <c r="G250" s="37"/>
-      <c r="H250" s="23">
-        <v>506</v>
-      </c>
-      <c r="I250" s="30" t="s">
-        <v>980</v>
-      </c>
-      <c r="J250" s="32" t="s">
-        <v>981</v>
-      </c>
-      <c r="K250" s="32"/>
-      <c r="L250" s="32"/>
-      <c r="M250" s="32"/>
-      <c r="N250" s="32"/>
-      <c r="O250" s="32"/>
-      <c r="P250" s="22"/>
-      <c r="Q250" s="22"/>
-      <c r="R250" s="22"/>
+      <c r="P250" s="40"/>
+      <c r="R250" s="40"/>
     </row>
     <row r="251" ht="14.25" customHeight="1" spans="1:18">
       <c r="A251" s="19">
         <v>245</v>
       </c>
       <c r="B251" s="24" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C251" s="25" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D251" s="22"/>
       <c r="E251" s="22"/>
@@ -12822,10 +12801,10 @@
         <v>246</v>
       </c>
       <c r="B252" s="24" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C252" s="25" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D252" s="22"/>
       <c r="E252" s="22"/>
@@ -12839,10 +12818,10 @@
         <v>247</v>
       </c>
       <c r="B253" s="24" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C253" s="25" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D253" s="22"/>
       <c r="E253" s="22"/>
@@ -12853,15 +12832,15 @@
       </c>
       <c r="I253" s="38"/>
       <c r="J253" s="42" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="K253" s="42"/>
       <c r="L253" s="42" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="M253" s="42"/>
       <c r="N253" s="42" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="O253" s="42"/>
     </row>
@@ -12870,41 +12849,41 @@
         <v>248</v>
       </c>
       <c r="B254" s="24" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C254" s="25" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D254" s="22"/>
       <c r="E254" s="22"/>
       <c r="F254" s="22"/>
       <c r="G254" s="37"/>
       <c r="H254" s="39" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="I254" s="39"/>
       <c r="J254" s="43">
-        <f>SUM(D7:D268,P7:P249)</f>
+        <f>SUM(D7:D268,P7:P248)</f>
         <v>0</v>
       </c>
       <c r="K254" s="44">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L254" s="43">
-        <f>SUM(E7:E268,Q7:Q249)</f>
+        <f>SUM(E7:E268,Q7:Q248)</f>
         <v>0</v>
       </c>
       <c r="M254" s="45">
         <f>K254</f>
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="N254" s="43">
-        <f>SUM(F7:F268,R7:R249)</f>
+        <f>SUM(F7:F268,R7:R248)</f>
         <v>0</v>
       </c>
       <c r="O254" s="45">
         <f>M254</f>
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="255" ht="14.25" customHeight="1" spans="1:15">
@@ -12912,17 +12891,17 @@
         <v>249</v>
       </c>
       <c r="B255" s="24" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C255" s="25" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D255" s="22"/>
       <c r="E255" s="22"/>
       <c r="F255" s="22"/>
       <c r="G255" s="37"/>
       <c r="H255" s="39" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I255" s="39"/>
       <c r="J255" s="46">
@@ -12930,21 +12909,21 @@
         <v>100</v>
       </c>
       <c r="K255" s="45" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L255" s="46">
         <f>(M254-L254)/M254*100</f>
         <v>100</v>
       </c>
       <c r="M255" s="45" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="N255" s="46">
         <f>(O254-N254)/O254*100</f>
         <v>100</v>
       </c>
       <c r="O255" s="45" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="256" ht="14.25" customHeight="1" spans="1:7">
@@ -12952,10 +12931,10 @@
         <v>250</v>
       </c>
       <c r="B256" s="24" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C256" s="25" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D256" s="22"/>
       <c r="E256" s="22"/>
@@ -12967,10 +12946,10 @@
         <v>251</v>
       </c>
       <c r="B257" s="24" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="C257" s="25" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D257" s="22"/>
       <c r="E257" s="22"/>
@@ -12982,10 +12961,10 @@
         <v>252</v>
       </c>
       <c r="B258" s="24" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="C258" s="25" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D258" s="22"/>
       <c r="E258" s="22"/>
@@ -12997,10 +12976,10 @@
         <v>253</v>
       </c>
       <c r="B259" s="24" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C259" s="25" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="D259" s="22"/>
       <c r="E259" s="22"/>
@@ -13012,24 +12991,24 @@
         <v>254</v>
       </c>
       <c r="B260" s="24" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C260" s="25" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="D260" s="22"/>
       <c r="E260" s="22"/>
       <c r="F260" s="22"/>
       <c r="G260" s="15"/>
       <c r="H260" s="47" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="I260" s="47"/>
       <c r="J260" s="47"/>
       <c r="K260" s="47"/>
       <c r="L260" s="53"/>
       <c r="M260" s="47" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="N260" s="47"/>
       <c r="O260" s="47"/>
@@ -13040,10 +13019,10 @@
         <v>255</v>
       </c>
       <c r="B261" s="24" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C261" s="25" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="D261" s="22"/>
       <c r="E261" s="22"/>
@@ -13064,10 +13043,10 @@
         <v>256</v>
       </c>
       <c r="B262" s="24" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C262" s="25" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="D262" s="22"/>
       <c r="E262" s="22"/>
@@ -13088,10 +13067,10 @@
         <v>257</v>
       </c>
       <c r="B263" s="24" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="C263" s="25" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="D263" s="22"/>
       <c r="E263" s="22"/>
@@ -13112,10 +13091,10 @@
         <v>258</v>
       </c>
       <c r="B264" s="24" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="C264" s="25" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="D264" s="22"/>
       <c r="E264" s="22"/>
@@ -13136,10 +13115,10 @@
         <v>259</v>
       </c>
       <c r="B265" s="24" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="C265" s="25" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="D265" s="22"/>
       <c r="E265" s="22"/>
@@ -13160,17 +13139,17 @@
         <v>260</v>
       </c>
       <c r="B266" s="49" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C266" s="25" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D266" s="22"/>
       <c r="E266" s="22"/>
       <c r="F266" s="22"/>
       <c r="G266" s="15"/>
       <c r="H266" s="50" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="I266" s="50"/>
       <c r="J266" s="50"/>
@@ -13186,10 +13165,10 @@
         <v>261</v>
       </c>
       <c r="B267" s="49" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="C267" s="25" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="D267" s="22"/>
       <c r="E267" s="22"/>
@@ -13210,10 +13189,10 @@
         <v>262</v>
       </c>
       <c r="B268" s="49" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="C268" s="25" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="D268" s="22"/>
       <c r="E268" s="22"/>
@@ -30673,7 +30652,7 @@
       <c r="S1137" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="264">
+  <mergeCells count="263">
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="A3:C3"/>
@@ -30922,7 +30901,6 @@
     <mergeCell ref="J247:O247"/>
     <mergeCell ref="J248:O248"/>
     <mergeCell ref="J249:O249"/>
-    <mergeCell ref="J250:O250"/>
     <mergeCell ref="H253:I253"/>
     <mergeCell ref="J253:K253"/>
     <mergeCell ref="L253:M253"/>
@@ -30965,7 +30943,7 @@
   <sheetData>
     <row r="1" ht="36.75" customHeight="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -30985,7 +30963,7 @@
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -31005,16 +30983,16 @@
     </row>
     <row r="24" spans="3:13">
       <c r="C24" s="3" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="25" spans="3:13">
       <c r="C25" s="3"/>
       <c r="M25" s="3" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="26" spans="3:13">
@@ -31027,13 +31005,13 @@
     </row>
     <row r="28" spans="3:13">
       <c r="C28" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="13:13">
       <c r="M29" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>